<commit_message>
Version du plan de test pour la revue 2. Il reste quelques tests à définir, mais les fonctions importantes sont avancées ou finalisées.
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Plans de test logiciel revue 2.xlsx
+++ b/Documentation/Tests/Plans de test logiciel revue 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paranize\Documents\UdS\S5\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paranize\Documents\UdS\S5\Projet\GIT\Documentation\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Personne responsable:</t>
   </si>
@@ -238,6 +238,45 @@
   </si>
   <si>
     <t>Le programme rentre dans l'interruption lorsque les conditions sont atteintes</t>
+  </si>
+  <si>
+    <t>Vérifier la quantification des  données de l'ADC</t>
+  </si>
+  <si>
+    <t>Les données de l'ADC sont dans la notation Q prévue</t>
+  </si>
+  <si>
+    <t>Envoyer un signal sinusoïdal de 1kHz</t>
+  </si>
+  <si>
+    <t>Le signal à la sortie est un sinus de 1kHz</t>
+  </si>
+  <si>
+    <t>Harmonizer</t>
+  </si>
+  <si>
+    <t>Passer en entrée un signal dont la fondamentale est connue. (ex:sinus pure)</t>
+  </si>
+  <si>
+    <t>Obtenir comme réponse à la FFT cette fondamentale.</t>
+  </si>
+  <si>
+    <t>Vérifier l'alignement des tableaux</t>
+  </si>
+  <si>
+    <t>Les tableaux sont aligné sur des frontières de double word</t>
+  </si>
+  <si>
+    <t>Vérifier la taille des tableaux</t>
+  </si>
+  <si>
+    <t>Les tableaux sont assez grand pour acqueillir toutes les données ainsi que la partie Im</t>
+  </si>
+  <si>
+    <t>Vérifier à l'oscilloscope le signal à la sortie de l'harmoniseur</t>
+  </si>
+  <si>
+    <t>Le signal des sortie se trouve un octave plus haut que le signal d'entrée</t>
   </si>
 </sst>
 </file>
@@ -261,7 +300,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="64">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -1070,11 +1109,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1109,6 +1157,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1201,202 +1309,184 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1405,35 +1495,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1446,15 +1524,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1790,16 +1859,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-      <c r="F2" s="37" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="F2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="60"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -1808,16 +1877,16 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44"/>
-      <c r="F3" s="41" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="64"/>
+      <c r="F3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="45"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -1826,22 +1895,22 @@
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="45" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="14" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1856,181 +1925,181 @@
       <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="29"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="49"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="O6" s="32"/>
+      <c r="O6" s="52"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="31"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="51"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="O7" s="33"/>
+      <c r="O7" s="53"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="31"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="51"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="33"/>
+      <c r="O8" s="53"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="31"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="51"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="O9" s="33"/>
+      <c r="O9" s="53"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="31"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="51"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="O10" s="33"/>
+      <c r="O10" s="53"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="31"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="51"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="O11" s="33"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="31"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="51"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="O12" s="33"/>
+      <c r="O12" s="53"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="31"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="51"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="O13" s="33"/>
+      <c r="O13" s="53"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>9</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="31"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="51"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="O14" s="33"/>
+      <c r="O14" s="53"/>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="45"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="O15" s="34"/>
+      <c r="O15" s="54"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -2095,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,16 +2182,16 @@
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="36"/>
-      <c r="F2" s="37" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="F2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="40"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="60"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2131,16 +2200,16 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="44"/>
-      <c r="F3" s="41" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="64"/>
+      <c r="F3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="45"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -2149,22 +2218,22 @@
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="45" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="14" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="16"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
       <c r="L5" s="13" t="s">
         <v>7</v>
       </c>
@@ -2176,821 +2245,859 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80">
+      <c r="A6" s="20">
         <v>1</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="44"/>
-      <c r="O6" s="32"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="64"/>
+      <c r="O6" s="52"/>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53">
+      <c r="A7" s="14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="46" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="29"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="49"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c r="O7" s="33"/>
+      <c r="O7" s="53"/>
     </row>
     <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54">
+      <c r="A8" s="15">
         <v>1.2</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="47" t="s">
+      <c r="C8" s="41"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="31"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="51"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="33"/>
+      <c r="O8" s="53"/>
     </row>
     <row r="9" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54">
+      <c r="A9" s="15">
         <v>1.3</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="55" t="s">
+      <c r="C9" s="41"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="51"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="31"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="51"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="O9" s="33"/>
+      <c r="O9" s="53"/>
     </row>
     <row r="10" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54">
+      <c r="A10" s="15">
         <v>1.4</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="55" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="51"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="31"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="51"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="O10" s="33"/>
+      <c r="O10" s="53"/>
     </row>
     <row r="11" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54">
+      <c r="A11" s="15">
         <v>1.5</v>
       </c>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="47" t="s">
+      <c r="C11" s="41"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="31"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="51"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="O11" s="33"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="54">
+      <c r="A12" s="15">
         <v>1.6</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="55" t="s">
+      <c r="C12" s="41"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="56"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="31"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="51"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="O12" s="33"/>
+      <c r="O12" s="53"/>
     </row>
     <row r="13" spans="1:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="81">
+      <c r="A13" s="21">
         <v>1.7</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="63"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="65" t="s">
+      <c r="C13" s="84"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="69"/>
-      <c r="O13" s="33"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="84"/>
+      <c r="J13" s="84"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="O13" s="53"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="80">
+      <c r="A14" s="20">
         <v>2</v>
       </c>
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="76"/>
-      <c r="O14" s="33"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="82"/>
+      <c r="O14" s="53"/>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="83">
+      <c r="A15" s="22">
         <v>2.1</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="75" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="85"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="82" t="s">
+      <c r="C15" s="76"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
-      <c r="O15" s="34"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="O15" s="54"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="89">
+      <c r="A16" s="24">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B16" s="87" t="s">
+      <c r="B16" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="62" t="s">
+      <c r="C16" s="84"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="63"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="68"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="88"/>
-      <c r="M16" s="88"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="89"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="85"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
       <c r="O16" s="2"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="80">
+      <c r="A17" s="20">
         <v>3</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="44"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="64"/>
     </row>
     <row r="18" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53">
+      <c r="A18" s="14">
         <v>3.1</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="29"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="52"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="29"/>
+      <c r="F18" s="91"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="49"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
     <row r="19" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="54">
+      <c r="A19" s="15">
         <v>3.2</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="55" t="s">
+      <c r="C19" s="41"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="51"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="31"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="54">
+      <c r="A20" s="15">
         <v>3.3</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="55" t="s">
+      <c r="C20" s="41"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="31"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="51"/>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="81">
+      <c r="A21" s="21">
         <v>3.4</v>
       </c>
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="93"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="99" t="s">
+      <c r="C21" s="104"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="100"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="110"/>
+      <c r="K21" s="111"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
     </row>
     <row r="22" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="81">
+      <c r="A22" s="21">
         <v>3.5</v>
       </c>
-      <c r="B22" s="102" t="s">
+      <c r="B22" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="103"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="102" t="s">
+      <c r="C22" s="98"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="103"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="106"/>
-      <c r="J22" s="106"/>
-      <c r="K22" s="107"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="69"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="101"/>
+      <c r="J22" s="101"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
     </row>
     <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="98">
+      <c r="A23" s="25">
         <v>4</v>
       </c>
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="97"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="95"/>
+      <c r="J23" s="95"/>
+      <c r="K23" s="95"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="96"/>
     </row>
     <row r="24" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="53">
+      <c r="A24" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="29"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="52"/>
-      <c r="G24" s="91"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="29"/>
+      <c r="F24" s="91"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="49"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="54">
+      <c r="A25" s="15">
         <v>4.2</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="B25" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="31"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="51"/>
       <c r="E25" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="52"/>
-      <c r="G25" s="91"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="31"/>
+      <c r="F25" s="91"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="51"/>
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
     </row>
     <row r="26" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54">
+      <c r="A26" s="15">
         <v>4.3</v>
       </c>
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="55" t="s">
+      <c r="C26" s="41"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="51"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="31"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="51"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
     </row>
     <row r="27" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54">
+      <c r="A27" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="55" t="s">
+      <c r="C27" s="41"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="51"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="31"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="51"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
     </row>
     <row r="28" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="81">
+      <c r="A28" s="21">
         <v>4.5</v>
       </c>
-      <c r="B28" s="92" t="s">
+      <c r="B28" s="103" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="93"/>
-      <c r="D28" s="94"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="105"/>
       <c r="E28" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="52"/>
-      <c r="G28" s="91"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="110"/>
+      <c r="J28" s="110"/>
+      <c r="K28" s="111"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="81">
+      <c r="A29" s="21">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="103" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="93"/>
-      <c r="D29" s="94"/>
-      <c r="E29" s="55" t="s">
+      <c r="C29" s="104"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="51"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="110"/>
+      <c r="J29" s="110"/>
+      <c r="K29" s="111"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
     </row>
     <row r="30" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="81">
+      <c r="A30" s="21">
         <v>4.7</v>
       </c>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="55" t="s">
+      <c r="C30" s="41"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="51"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="109"/>
+      <c r="I30" s="110"/>
+      <c r="J30" s="110"/>
+      <c r="K30" s="111"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
     </row>
     <row r="31" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="81">
+      <c r="A31" s="21">
         <v>4.8</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="55" t="s">
+      <c r="C31" s="41"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="51"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="110"/>
+      <c r="J31" s="110"/>
+      <c r="K31" s="111"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
     </row>
     <row r="32" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="81">
+      <c r="A32" s="21">
         <v>4.9000000000000004</v>
       </c>
-      <c r="B32" s="92" t="s">
+      <c r="B32" s="103" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="93"/>
-      <c r="D32" s="94"/>
+      <c r="C32" s="104"/>
+      <c r="D32" s="105"/>
       <c r="E32" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="52"/>
-      <c r="G32" s="91"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
+      <c r="F32" s="91"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="110"/>
+      <c r="J32" s="110"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
     </row>
     <row r="33" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="108">
+      <c r="A33" s="26">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="93"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="55" t="s">
+      <c r="C33" s="104"/>
+      <c r="D33" s="105"/>
+      <c r="E33" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="51"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="110"/>
+      <c r="J33" s="110"/>
+      <c r="K33" s="111"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
     </row>
     <row r="34" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="81">
+      <c r="A34" s="21">
         <v>4.1100000000000003</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="55" t="s">
+      <c r="C34" s="41"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="69" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="51"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="69"/>
-      <c r="M34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="110"/>
+      <c r="J34" s="110"/>
+      <c r="K34" s="111"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
     </row>
     <row r="35" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="123">
+      <c r="A35" s="29">
         <v>4.12</v>
       </c>
-      <c r="B35" s="112" t="s">
+      <c r="B35" s="126" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="113"/>
-      <c r="E35" s="65" t="s">
+      <c r="C35" s="87"/>
+      <c r="D35" s="127"/>
+      <c r="E35" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="66"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="105"/>
-      <c r="I35" s="106"/>
-      <c r="J35" s="106"/>
-      <c r="K35" s="107"/>
-      <c r="L35" s="69"/>
-      <c r="M35" s="69"/>
+      <c r="F35" s="87"/>
+      <c r="G35" s="127"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="101"/>
+      <c r="J35" s="101"/>
+      <c r="K35" s="102"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
     </row>
     <row r="36" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="98">
+      <c r="A36" s="25">
         <v>5</v>
       </c>
-      <c r="B36" s="109" t="s">
+      <c r="B36" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="110"/>
-      <c r="D36" s="110"/>
-      <c r="E36" s="110"/>
-      <c r="F36" s="110"/>
-      <c r="G36" s="110"/>
-      <c r="H36" s="110"/>
-      <c r="I36" s="110"/>
-      <c r="J36" s="110"/>
-      <c r="K36" s="110"/>
-      <c r="L36" s="110"/>
-      <c r="M36" s="111"/>
+      <c r="C36" s="120"/>
+      <c r="D36" s="120"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="120"/>
+      <c r="G36" s="120"/>
+      <c r="H36" s="120"/>
+      <c r="I36" s="120"/>
+      <c r="J36" s="120"/>
+      <c r="K36" s="120"/>
+      <c r="L36" s="120"/>
+      <c r="M36" s="121"/>
     </row>
     <row r="37" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="129">
+      <c r="A37" s="31">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B37" s="124" t="s">
+      <c r="B37" s="134" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="125"/>
-      <c r="D37" s="126"/>
-      <c r="E37" s="124" t="s">
+      <c r="C37" s="135"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="134" t="s">
         <v>61</v>
       </c>
-      <c r="F37" s="125"/>
-      <c r="G37" s="126"/>
-      <c r="H37" s="127"/>
-      <c r="I37" s="127"/>
-      <c r="J37" s="127"/>
-      <c r="K37" s="127"/>
-      <c r="L37" s="128"/>
-      <c r="M37" s="130" t="s">
+      <c r="F37" s="135"/>
+      <c r="G37" s="136"/>
+      <c r="H37" s="137"/>
+      <c r="I37" s="137"/>
+      <c r="J37" s="137"/>
+      <c r="K37" s="137"/>
+      <c r="L37" s="30"/>
+      <c r="M37" s="32" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="122">
+      <c r="A38" s="28">
         <v>5.2</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="123" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="118"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="50" t="s">
+      <c r="C38" s="124"/>
+      <c r="D38" s="125"/>
+      <c r="E38" s="123" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="118"/>
-      <c r="G38" s="119"/>
-      <c r="H38" s="120"/>
-      <c r="I38" s="120"/>
-      <c r="J38" s="120"/>
-      <c r="K38" s="120"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="69"/>
-    </row>
-    <row r="39" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="122">
+      <c r="F38" s="124"/>
+      <c r="G38" s="125"/>
+      <c r="H38" s="122"/>
+      <c r="I38" s="122"/>
+      <c r="J38" s="122"/>
+      <c r="K38" s="122"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="16"/>
+    </row>
+    <row r="39" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28">
         <v>5.3</v>
       </c>
-      <c r="B39" s="50"/>
-      <c r="C39" s="118"/>
-      <c r="D39" s="119"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="118"/>
-      <c r="G39" s="119"/>
-      <c r="H39" s="120"/>
-      <c r="I39" s="120"/>
-      <c r="J39" s="120"/>
-      <c r="K39" s="120"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="69"/>
-    </row>
-    <row r="40" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="122"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="100"/>
-      <c r="D40" s="101"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="100"/>
-      <c r="G40" s="101"/>
-      <c r="H40" s="57"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="69"/>
-    </row>
-    <row r="41" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="122"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="100"/>
-      <c r="D41" s="101"/>
-      <c r="E41" s="99"/>
-      <c r="F41" s="100"/>
-      <c r="G41" s="101"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="59"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="69"/>
+      <c r="B39" s="123" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="124"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="123" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="124"/>
+      <c r="G39" s="125"/>
+      <c r="H39" s="122"/>
+      <c r="I39" s="122"/>
+      <c r="J39" s="122"/>
+      <c r="K39" s="122"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="16"/>
+    </row>
+    <row r="40" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="29">
+        <v>5.4</v>
+      </c>
+      <c r="B40" s="97" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="98"/>
+      <c r="D40" s="99"/>
+      <c r="E40" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="98"/>
+      <c r="G40" s="99"/>
+      <c r="H40" s="100"/>
+      <c r="I40" s="101"/>
+      <c r="J40" s="101"/>
+      <c r="K40" s="102"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="16"/>
+    </row>
+    <row r="41" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="25">
+        <v>6</v>
+      </c>
+      <c r="B41" s="119" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="120"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
+      <c r="G41" s="120"/>
+      <c r="H41" s="120"/>
+      <c r="I41" s="120"/>
+      <c r="J41" s="120"/>
+      <c r="K41" s="120"/>
+      <c r="L41" s="120"/>
+      <c r="M41" s="121"/>
     </row>
     <row r="42" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="122"/>
-      <c r="B42" s="99"/>
-      <c r="C42" s="100"/>
-      <c r="D42" s="101"/>
-      <c r="E42" s="99"/>
-      <c r="F42" s="100"/>
-      <c r="G42" s="101"/>
-      <c r="H42" s="57"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="79"/>
-      <c r="M42" s="69"/>
+      <c r="A42" s="31">
+        <v>6.1</v>
+      </c>
+      <c r="B42" s="131" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="132"/>
+      <c r="D42" s="133"/>
+      <c r="E42" s="131" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" s="132"/>
+      <c r="G42" s="133"/>
+      <c r="H42" s="128"/>
+      <c r="I42" s="129"/>
+      <c r="J42" s="129"/>
+      <c r="K42" s="130"/>
+      <c r="L42" s="30"/>
+      <c r="M42" s="33"/>
     </row>
     <row r="43" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="122"/>
-      <c r="B43" s="99"/>
-      <c r="C43" s="100"/>
-      <c r="D43" s="101"/>
-      <c r="E43" s="99"/>
-      <c r="F43" s="100"/>
-      <c r="G43" s="101"/>
-      <c r="H43" s="57"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="59"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="69"/>
+      <c r="A43" s="28">
+        <v>6.2</v>
+      </c>
+      <c r="B43" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43" s="107"/>
+      <c r="D43" s="108"/>
+      <c r="E43" s="106" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="107"/>
+      <c r="G43" s="108"/>
+      <c r="H43" s="109"/>
+      <c r="I43" s="110"/>
+      <c r="J43" s="110"/>
+      <c r="K43" s="111"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="16"/>
     </row>
     <row r="44" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="122"/>
-      <c r="B44" s="99"/>
-      <c r="C44" s="100"/>
-      <c r="D44" s="101"/>
-      <c r="E44" s="99"/>
-      <c r="F44" s="100"/>
-      <c r="G44" s="101"/>
-      <c r="H44" s="57"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
-      <c r="K44" s="59"/>
-      <c r="L44" s="79"/>
-      <c r="M44" s="69"/>
+      <c r="A44" s="28">
+        <v>6.3</v>
+      </c>
+      <c r="B44" s="131" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="132"/>
+      <c r="D44" s="133"/>
+      <c r="E44" s="131" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" s="132"/>
+      <c r="G44" s="133"/>
+      <c r="H44" s="109"/>
+      <c r="I44" s="110"/>
+      <c r="J44" s="110"/>
+      <c r="K44" s="111"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="16"/>
     </row>
     <row r="45" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="122"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="118"/>
-      <c r="D45" s="119"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="118"/>
-      <c r="G45" s="119"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="120"/>
-      <c r="J45" s="120"/>
-      <c r="K45" s="120"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="69"/>
+      <c r="A45" s="28">
+        <v>6.4</v>
+      </c>
+      <c r="B45" s="123" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="124"/>
+      <c r="D45" s="125"/>
+      <c r="E45" s="123" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="124"/>
+      <c r="G45" s="125"/>
+      <c r="H45" s="122"/>
+      <c r="I45" s="122"/>
+      <c r="J45" s="122"/>
+      <c r="K45" s="122"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="16"/>
     </row>
     <row r="46" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="121"/>
-      <c r="B46" s="114"/>
-      <c r="C46" s="115"/>
-      <c r="D46" s="116"/>
-      <c r="E46" s="117"/>
-      <c r="F46" s="115"/>
-      <c r="G46" s="116"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="71"/>
-      <c r="J46" s="71"/>
-      <c r="K46" s="72"/>
-      <c r="L46" s="73"/>
+      <c r="A46" s="27"/>
+      <c r="B46" s="112"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="114"/>
+      <c r="E46" s="115"/>
+      <c r="F46" s="113"/>
+      <c r="G46" s="114"/>
+      <c r="H46" s="116"/>
+      <c r="I46" s="117"/>
+      <c r="J46" s="117"/>
+      <c r="K46" s="118"/>
+      <c r="L46" s="17"/>
       <c r="M46" s="6"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -3020,22 +3127,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="123">
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B36:M36"/>
-    <mergeCell ref="H41:K41"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B42:D42"/>
+  <mergeCells count="121">
     <mergeCell ref="E38:G38"/>
     <mergeCell ref="E37:G37"/>
     <mergeCell ref="B38:D38"/>
@@ -3044,6 +3136,7 @@
     <mergeCell ref="H37:K37"/>
     <mergeCell ref="H38:K38"/>
     <mergeCell ref="H39:K39"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="H45:K45"/>
     <mergeCell ref="E45:G45"/>
     <mergeCell ref="B45:D45"/>
@@ -3055,6 +3148,29 @@
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="H35:K35"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B36:M36"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B41:M41"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="H32:K32"/>
@@ -3068,17 +3184,6 @@
     <mergeCell ref="H30:K30"/>
     <mergeCell ref="H31:K31"/>
     <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="H25:K25"/>
@@ -3098,6 +3203,8 @@
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="H21:K21"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:K13"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="H18:K18"/>
@@ -3108,16 +3215,6 @@
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:K13"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="H10:K10"/>
@@ -3134,6 +3231,14 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="H9:K9"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:K5"/>

</xml_diff>

<commit_message>
test de fréquence de coupure matlab
</commit_message>
<xml_diff>
--- a/Documentation/Tests/Plans de test logiciel revue 2.xlsx
+++ b/Documentation/Tests/Plans de test logiciel revue 2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paranize\Documents\UdS\S5\Projet\GIT\Documentation\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olaberge\Documents\S5\Projet S5\Repo_Projet_S5\Documentation\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69E96B7-3890-473C-A1D5-B2350FC01C31}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gabarit" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="94">
   <si>
     <t>Personne responsable:</t>
   </si>
@@ -277,12 +278,63 @@
   </si>
   <si>
     <t>Le signal des sortie se trouve un octave plus haut que le signal d'entrée</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>1.2.2</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>Filtre passe-bas 700 Hz</t>
+  </si>
+  <si>
+    <t>Filtre passe-haut 5000 kHz</t>
+  </si>
+  <si>
+    <t>Filtre passe-bas 1000 Hz</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>Filtre passe-bas 7000 Hz</t>
+  </si>
+  <si>
+    <t>Réussite</t>
+  </si>
+  <si>
+    <t>0.1426 rad normalisé</t>
+  </si>
+  <si>
+    <t>0.9973 rad normalisé</t>
+  </si>
+  <si>
+    <t>Fréquence de coupure à 700 Hz (0.0997331 rad normalisé)</t>
+  </si>
+  <si>
+    <t>Fréquence de coupure à 1000 Hz (0.14247585 rad normalisé)</t>
+  </si>
+  <si>
+    <t>Fréquence de coupure à 5000 Hz (0.712379287 rad normalisé)</t>
+  </si>
+  <si>
+    <t>Fréquence de coupure à 7000 Hz (0.997331001 rad normalisé)</t>
+  </si>
+  <si>
+    <t>0.7121 rad normalisé</t>
+  </si>
+  <si>
+    <t>0.0996 rad normalisé</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1122,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1217,60 +1269,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1300,19 +1298,100 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1327,12 +1406,150 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1360,170 +1577,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1838,79 +1899,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.7109375" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="12" max="12" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.7265625" customWidth="1"/>
+    <col min="15" max="15" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="F2" s="57" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="F2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="60"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="64"/>
-      <c r="F3" s="61" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="F3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="62"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="65" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="34" t="s">
+      <c r="F5" s="54"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="36"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="58"/>
       <c r="L5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1921,199 +1982,223 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="49"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="61"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
-      <c r="O6" s="52"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O6" s="34"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>2</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="51"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
       <c r="K7" s="51"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="O7" s="53"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O7" s="35"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>3</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="41"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="51"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="51"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="53"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O8" s="35"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="41"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
       <c r="D9" s="51"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
       <c r="K9" s="51"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="O9" s="53"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O9" s="35"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="41"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
       <c r="D10" s="51"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
       <c r="K10" s="51"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="O10" s="53"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O10" s="35"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="41"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="51"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
       <c r="K11" s="51"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
-      <c r="O11" s="53"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O11" s="35"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="41"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="51"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
       <c r="K12" s="51"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
-      <c r="O12" s="53"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O12" s="35"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="41"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="51"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
       <c r="K13" s="51"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
-      <c r="O13" s="53"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O13" s="35"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>9</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="41"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="51"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
       <c r="K14" s="51"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
-      <c r="O14" s="53"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O14" s="35"/>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="45"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="46"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="O15" s="54"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="O15" s="36"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="O6:O15"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -2130,30 +2215,6 @@
     <mergeCell ref="E13:G13"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2161,79 +2222,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="31.7109375" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
+    <col min="12" max="12" width="18.54296875" customWidth="1"/>
+    <col min="13" max="13" width="31.7265625" customWidth="1"/>
+    <col min="15" max="15" width="29.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="F2" s="57" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="F2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="58"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="60"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="64"/>
-      <c r="F3" s="61" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="F3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="62"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="65" t="s">
+      <c r="C5" s="54"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="34" t="s">
+      <c r="F5" s="54"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="36"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="58"/>
       <c r="L5" s="13" t="s">
         <v>7</v>
       </c>
@@ -2244,1001 +2305,1006 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="20">
         <v>1</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="67"/>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-      <c r="M6" s="64"/>
-      <c r="O6" s="52"/>
-    </row>
-    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+      <c r="K6" s="127"/>
+      <c r="L6" s="127"/>
+      <c r="M6" s="48"/>
+      <c r="O6" s="34"/>
+    </row>
+    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="74" t="s">
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="49"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="61"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c r="O7" s="53"/>
-    </row>
-    <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="35"/>
+    </row>
+    <row r="8" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="15">
         <v>1.2</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="41"/>
+      <c r="C8" s="50"/>
       <c r="D8" s="51"/>
-      <c r="E8" s="72" t="s">
+      <c r="E8" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
       <c r="K8" s="51"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="O8" s="53"/>
-    </row>
-    <row r="9" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="O8" s="35"/>
+    </row>
+    <row r="9" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="101"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="101"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="138"/>
+      <c r="J9" s="138"/>
+      <c r="K9" s="139"/>
+      <c r="L9" s="140" t="s">
+        <v>85</v>
+      </c>
+      <c r="M9" s="140"/>
+      <c r="O9" s="35"/>
+    </row>
+    <row r="10" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="100" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="101"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="101"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="100" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="138"/>
+      <c r="J10" s="138"/>
+      <c r="K10" s="139"/>
+      <c r="L10" s="140" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" s="140"/>
+      <c r="O10" s="35"/>
+    </row>
+    <row r="11" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="101"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="101"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="100" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="138"/>
+      <c r="J11" s="138"/>
+      <c r="K11" s="139"/>
+      <c r="L11" s="140" t="s">
+        <v>85</v>
+      </c>
+      <c r="M11" s="140"/>
+      <c r="O11" s="35"/>
+    </row>
+    <row r="12" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="100" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="101"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="100" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="101"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="100" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" s="138"/>
+      <c r="J12" s="138"/>
+      <c r="K12" s="139"/>
+      <c r="L12" s="140" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" s="140"/>
+      <c r="O12" s="35"/>
+    </row>
+    <row r="13" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="15">
         <v>1.3</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B13" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="69" t="s">
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="O9" s="53"/>
-    </row>
-    <row r="10" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="F13" s="79"/>
+      <c r="G13" s="80"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="O13" s="35"/>
+    </row>
+    <row r="14" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="15">
         <v>1.4</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B14" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="69" t="s">
+      <c r="C14" s="50"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="70"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="O10" s="53"/>
-    </row>
-    <row r="11" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="F14" s="79"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="O14" s="35"/>
+    </row>
+    <row r="15" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="15">
         <v>1.5</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B15" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="72" t="s">
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="O11" s="53"/>
-    </row>
-    <row r="12" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="F15" s="50"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="O15" s="35"/>
+    </row>
+    <row r="16" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="15">
         <v>1.6</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B16" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="69" t="s">
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="70"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="O12" s="53"/>
-    </row>
-    <row r="13" spans="1:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
+      <c r="F16" s="79"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="O16" s="35"/>
+    </row>
+    <row r="17" spans="1:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="21">
         <v>1.7</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B17" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="84"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="86" t="s">
+      <c r="C17" s="122"/>
+      <c r="D17" s="123"/>
+      <c r="E17" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="87"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="O13" s="53"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="20">
+      <c r="F17" s="85"/>
+      <c r="G17" s="120"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="122"/>
+      <c r="J17" s="122"/>
+      <c r="K17" s="123"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="O17" s="35"/>
+    </row>
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="20">
         <v>2</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="B18" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="82"/>
-      <c r="O14" s="53"/>
-    </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22">
+      <c r="C18" s="136"/>
+      <c r="D18" s="136"/>
+      <c r="E18" s="136"/>
+      <c r="F18" s="136"/>
+      <c r="G18" s="136"/>
+      <c r="H18" s="136"/>
+      <c r="I18" s="136"/>
+      <c r="J18" s="136"/>
+      <c r="K18" s="136"/>
+      <c r="L18" s="136"/>
+      <c r="M18" s="137"/>
+      <c r="O18" s="35"/>
+    </row>
+    <row r="19" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="22">
         <v>2.1</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B19" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="78" t="s">
+      <c r="C19" s="131"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="133" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="59"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="O15" s="54"/>
-    </row>
-    <row r="16" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="24">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B16" s="93" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="84"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="83" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="89"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="85"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="O16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20">
-        <v>3</v>
-      </c>
-      <c r="B17" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="64"/>
-    </row>
-    <row r="18" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
-        <v>3.1</v>
-      </c>
-      <c r="B18" s="73" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="90" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="91"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
-        <v>3.2</v>
-      </c>
-      <c r="B19" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="70"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="50"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="134"/>
       <c r="I19" s="41"/>
       <c r="J19" s="41"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="K19" s="42"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="O19" s="36"/>
+    </row>
+    <row r="20" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B20" s="124" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="122"/>
+      <c r="D20" s="123"/>
+      <c r="E20" s="125" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="122"/>
+      <c r="G20" s="123"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="122"/>
+      <c r="J20" s="122"/>
+      <c r="K20" s="123"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="20">
+        <v>3</v>
+      </c>
+      <c r="B21" s="126" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="127"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="127"/>
+      <c r="F21" s="127"/>
+      <c r="G21" s="127"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="127"/>
+      <c r="J21" s="127"/>
+      <c r="K21" s="127"/>
+      <c r="L21" s="127"/>
+      <c r="M21" s="48"/>
+    </row>
+    <row r="22" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14">
+        <v>3.1</v>
+      </c>
+      <c r="B22" s="116" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="60"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="113" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="114"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+    </row>
+    <row r="23" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="15">
+        <v>3.2</v>
+      </c>
+      <c r="B23" s="77" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="50"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="79"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="15">
         <v>3.3</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B24" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="69" t="s">
+      <c r="C24" s="50"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="70"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="F24" s="79"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="21">
         <v>3.4</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B25" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="104"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="106" t="s">
+      <c r="C25" s="111"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="F21" s="107"/>
-      <c r="G21" s="108"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="110"/>
-      <c r="K21" s="111"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-    </row>
-    <row r="22" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21">
+      <c r="F25" s="101"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="81"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="83"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+    </row>
+    <row r="26" spans="1:15" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="21">
         <v>3.5</v>
       </c>
-      <c r="B22" s="97" t="s">
+      <c r="B26" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="98"/>
-      <c r="D22" s="99"/>
-      <c r="E22" s="97" t="s">
+      <c r="C26" s="89"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="98"/>
-      <c r="G22" s="99"/>
-      <c r="H22" s="100"/>
-      <c r="I22" s="101"/>
-      <c r="J22" s="101"/>
-      <c r="K22" s="102"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="16"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25">
+      <c r="F26" s="89"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="73"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="25">
         <v>4</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="B27" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95"/>
-      <c r="F23" s="95"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
-      <c r="J23" s="95"/>
-      <c r="K23" s="95"/>
-      <c r="L23" s="95"/>
-      <c r="M23" s="96"/>
-    </row>
-    <row r="24" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14">
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="118"/>
+      <c r="I27" s="118"/>
+      <c r="J27" s="118"/>
+      <c r="K27" s="118"/>
+      <c r="L27" s="118"/>
+      <c r="M27" s="119"/>
+    </row>
+    <row r="28" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="B28" s="116" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="90" t="s">
+      <c r="C28" s="60"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="91"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-    </row>
-    <row r="25" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="F28" s="114"/>
+      <c r="G28" s="115"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="61"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="15">
         <v>4.2</v>
       </c>
-      <c r="B25" s="68" t="s">
+      <c r="B29" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="90" t="s">
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="91"/>
-      <c r="G25" s="92"/>
-      <c r="H25" s="50"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-    </row>
-    <row r="26" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="F29" s="114"/>
+      <c r="G29" s="115"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="51"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="15">
         <v>4.3</v>
       </c>
-      <c r="B26" s="68" t="s">
+      <c r="B30" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="69" t="s">
+      <c r="C30" s="50"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="F26" s="70"/>
-      <c r="G26" s="71"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+      <c r="F30" s="79"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B31" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="69" t="s">
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="70"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-    </row>
-    <row r="28" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21">
+      <c r="F31" s="79"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="21">
         <v>4.5</v>
       </c>
-      <c r="B28" s="103" t="s">
+      <c r="B32" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="104"/>
-      <c r="D28" s="105"/>
-      <c r="E28" s="90" t="s">
+      <c r="C32" s="111"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="113" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="91"/>
-      <c r="G28" s="92"/>
-      <c r="H28" s="109"/>
-      <c r="I28" s="110"/>
-      <c r="J28" s="110"/>
-      <c r="K28" s="111"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-    </row>
-    <row r="29" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="B29" s="103" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="104"/>
-      <c r="D29" s="105"/>
-      <c r="E29" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="F29" s="70"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="109"/>
-      <c r="I29" s="110"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="111"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-    </row>
-    <row r="30" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21">
-        <v>4.7</v>
-      </c>
-      <c r="B30" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" s="70"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="110"/>
-      <c r="J30" s="110"/>
-      <c r="K30" s="111"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-    </row>
-    <row r="31" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21">
-        <v>4.8</v>
-      </c>
-      <c r="B31" s="68" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="70"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="109"/>
-      <c r="I31" s="110"/>
-      <c r="J31" s="110"/>
-      <c r="K31" s="111"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-    </row>
-    <row r="32" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="21">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="B32" s="103" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="104"/>
-      <c r="D32" s="105"/>
-      <c r="E32" s="90" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="91"/>
-      <c r="G32" s="92"/>
-      <c r="H32" s="109"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="110"/>
-      <c r="K32" s="111"/>
+      <c r="F32" s="114"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="81"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="83"/>
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
     </row>
-    <row r="33" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="26">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B33" s="103" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="104"/>
-      <c r="D33" s="105"/>
-      <c r="E33" s="69" t="s">
+    <row r="33" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B33" s="110" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="111"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="70"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="109"/>
-      <c r="I33" s="110"/>
-      <c r="J33" s="110"/>
-      <c r="K33" s="111"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="82"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="83"/>
       <c r="L33" s="16"/>
       <c r="M33" s="16"/>
     </row>
-    <row r="34" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="21">
-        <v>4.1100000000000003</v>
-      </c>
-      <c r="B34" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="41"/>
+        <v>4.7</v>
+      </c>
+      <c r="B34" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="50"/>
       <c r="D34" s="51"/>
-      <c r="E34" s="69" t="s">
+      <c r="E34" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="F34" s="70"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="110"/>
-      <c r="J34" s="110"/>
-      <c r="K34" s="111"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="82"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="83"/>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
     </row>
-    <row r="35" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="29">
-        <v>4.12</v>
-      </c>
-      <c r="B35" s="126" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="87"/>
-      <c r="D35" s="127"/>
-      <c r="E35" s="86" t="s">
+    <row r="35" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="21">
+        <v>4.8</v>
+      </c>
+      <c r="B35" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="87"/>
-      <c r="G35" s="127"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="101"/>
-      <c r="J35" s="101"/>
-      <c r="K35" s="102"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="82"/>
+      <c r="J35" s="82"/>
+      <c r="K35" s="83"/>
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
     </row>
-    <row r="36" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25">
+    <row r="36" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="21">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B36" s="110" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="111"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="113" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="114"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="81"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="83"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+    </row>
+    <row r="37" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="26">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B37" s="110" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="111"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="79"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="81"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+    </row>
+    <row r="38" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="21">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="B38" s="77" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="50"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="79"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="81"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="83"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+    </row>
+    <row r="39" spans="1:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="29">
+        <v>4.12</v>
+      </c>
+      <c r="B39" s="84" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="85"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="85"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="73"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="74"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+    </row>
+    <row r="40" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="25">
         <v>5</v>
       </c>
-      <c r="B36" s="119" t="s">
+      <c r="B40" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="120"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="120"/>
-      <c r="F36" s="120"/>
-      <c r="G36" s="120"/>
-      <c r="H36" s="120"/>
-      <c r="I36" s="120"/>
-      <c r="J36" s="120"/>
-      <c r="K36" s="120"/>
-      <c r="L36" s="120"/>
-      <c r="M36" s="121"/>
-    </row>
-    <row r="37" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="31">
+      <c r="C40" s="92"/>
+      <c r="D40" s="92"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="92"/>
+      <c r="H40" s="92"/>
+      <c r="I40" s="92"/>
+      <c r="J40" s="92"/>
+      <c r="K40" s="92"/>
+      <c r="L40" s="92"/>
+      <c r="M40" s="93"/>
+    </row>
+    <row r="41" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="31">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B37" s="134" t="s">
+      <c r="B41" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="135"/>
-      <c r="D37" s="136"/>
-      <c r="E37" s="134" t="s">
+      <c r="C41" s="70"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="F37" s="135"/>
-      <c r="G37" s="136"/>
-      <c r="H37" s="137"/>
-      <c r="I37" s="137"/>
-      <c r="J37" s="137"/>
-      <c r="K37" s="137"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="32" t="s">
+      <c r="F41" s="70"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="75"/>
+      <c r="J41" s="75"/>
+      <c r="K41" s="75"/>
+      <c r="L41" s="30"/>
+      <c r="M41" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28">
+    <row r="42" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="28">
         <v>5.2</v>
       </c>
-      <c r="B38" s="123" t="s">
+      <c r="B42" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="124"/>
-      <c r="D38" s="125"/>
-      <c r="E38" s="123" t="s">
+      <c r="C42" s="67"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="124"/>
-      <c r="G38" s="125"/>
-      <c r="H38" s="122"/>
-      <c r="I38" s="122"/>
-      <c r="J38" s="122"/>
-      <c r="K38" s="122"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="16"/>
-    </row>
-    <row r="39" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28">
+      <c r="F42" s="67"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="16"/>
+    </row>
+    <row r="43" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="28">
         <v>5.3</v>
       </c>
-      <c r="B39" s="123" t="s">
+      <c r="B43" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="124"/>
-      <c r="D39" s="125"/>
-      <c r="E39" s="123" t="s">
+      <c r="C43" s="67"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="124"/>
-      <c r="G39" s="125"/>
-      <c r="H39" s="122"/>
-      <c r="I39" s="122"/>
-      <c r="J39" s="122"/>
-      <c r="K39" s="122"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="16"/>
-    </row>
-    <row r="40" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="29">
-        <v>5.4</v>
-      </c>
-      <c r="B40" s="97" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="98"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="97" t="s">
-        <v>67</v>
-      </c>
-      <c r="F40" s="98"/>
-      <c r="G40" s="99"/>
-      <c r="H40" s="100"/>
-      <c r="I40" s="101"/>
-      <c r="J40" s="101"/>
-      <c r="K40" s="102"/>
-      <c r="L40" s="23"/>
-      <c r="M40" s="16"/>
-    </row>
-    <row r="41" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="25">
-        <v>6</v>
-      </c>
-      <c r="B41" s="119" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="120"/>
-      <c r="D41" s="120"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120"/>
-      <c r="G41" s="120"/>
-      <c r="H41" s="120"/>
-      <c r="I41" s="120"/>
-      <c r="J41" s="120"/>
-      <c r="K41" s="120"/>
-      <c r="L41" s="120"/>
-      <c r="M41" s="121"/>
-    </row>
-    <row r="42" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="31">
-        <v>6.1</v>
-      </c>
-      <c r="B42" s="131" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="132"/>
-      <c r="D42" s="133"/>
-      <c r="E42" s="131" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" s="132"/>
-      <c r="G42" s="133"/>
-      <c r="H42" s="128"/>
-      <c r="I42" s="129"/>
-      <c r="J42" s="129"/>
-      <c r="K42" s="130"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="33"/>
-    </row>
-    <row r="43" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="28">
-        <v>6.2</v>
-      </c>
-      <c r="B43" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="C43" s="107"/>
-      <c r="D43" s="108"/>
-      <c r="E43" s="106" t="s">
-        <v>74</v>
-      </c>
-      <c r="F43" s="107"/>
-      <c r="G43" s="108"/>
-      <c r="H43" s="109"/>
-      <c r="I43" s="110"/>
-      <c r="J43" s="110"/>
-      <c r="K43" s="111"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+      <c r="J43" s="76"/>
+      <c r="K43" s="76"/>
       <c r="L43" s="19"/>
       <c r="M43" s="16"/>
     </row>
-    <row r="44" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28">
+    <row r="44" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="29">
+        <v>5.4</v>
+      </c>
+      <c r="B44" s="88" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="89"/>
+      <c r="D44" s="90"/>
+      <c r="E44" s="88" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="89"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="73"/>
+      <c r="J44" s="73"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="16"/>
+    </row>
+    <row r="45" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="25">
+        <v>6</v>
+      </c>
+      <c r="B45" s="91" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="92"/>
+      <c r="D45" s="92"/>
+      <c r="E45" s="92"/>
+      <c r="F45" s="92"/>
+      <c r="G45" s="92"/>
+      <c r="H45" s="92"/>
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="92"/>
+      <c r="L45" s="92"/>
+      <c r="M45" s="93"/>
+    </row>
+    <row r="46" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="31">
+        <v>6.1</v>
+      </c>
+      <c r="B46" s="97" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="98"/>
+      <c r="D46" s="99"/>
+      <c r="E46" s="97" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" s="98"/>
+      <c r="G46" s="99"/>
+      <c r="H46" s="94"/>
+      <c r="I46" s="95"/>
+      <c r="J46" s="95"/>
+      <c r="K46" s="96"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="33"/>
+    </row>
+    <row r="47" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="28">
+        <v>6.2</v>
+      </c>
+      <c r="B47" s="100" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" s="101"/>
+      <c r="D47" s="102"/>
+      <c r="E47" s="100" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="101"/>
+      <c r="G47" s="102"/>
+      <c r="H47" s="81"/>
+      <c r="I47" s="82"/>
+      <c r="J47" s="82"/>
+      <c r="K47" s="83"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="16"/>
+    </row>
+    <row r="48" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="28">
         <v>6.3</v>
       </c>
-      <c r="B44" s="131" t="s">
+      <c r="B48" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="132"/>
-      <c r="D44" s="133"/>
-      <c r="E44" s="131" t="s">
+      <c r="C48" s="98"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="F44" s="132"/>
-      <c r="G44" s="133"/>
-      <c r="H44" s="109"/>
-      <c r="I44" s="110"/>
-      <c r="J44" s="110"/>
-      <c r="K44" s="111"/>
-      <c r="L44" s="19"/>
-      <c r="M44" s="16"/>
-    </row>
-    <row r="45" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28">
+      <c r="F48" s="98"/>
+      <c r="G48" s="99"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="82"/>
+      <c r="J48" s="82"/>
+      <c r="K48" s="83"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="16"/>
+    </row>
+    <row r="49" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="28">
         <v>6.4</v>
       </c>
-      <c r="B45" s="123" t="s">
+      <c r="B49" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="124"/>
-      <c r="D45" s="125"/>
-      <c r="E45" s="123" t="s">
+      <c r="C49" s="67"/>
+      <c r="D49" s="68"/>
+      <c r="E49" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="F45" s="124"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="122"/>
-      <c r="I45" s="122"/>
-      <c r="J45" s="122"/>
-      <c r="K45" s="122"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="16"/>
-    </row>
-    <row r="46" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27"/>
-      <c r="B46" s="112"/>
-      <c r="C46" s="113"/>
-      <c r="D46" s="114"/>
-      <c r="E46" s="115"/>
-      <c r="F46" s="113"/>
-      <c r="G46" s="114"/>
-      <c r="H46" s="116"/>
-      <c r="I46" s="117"/>
-      <c r="J46" s="117"/>
-      <c r="K46" s="118"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="6"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-    </row>
-    <row r="48" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+      <c r="F49" s="67"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="76"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="16"/>
+    </row>
+    <row r="50" spans="1:13" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="27"/>
+      <c r="B50" s="103"/>
+      <c r="C50" s="104"/>
+      <c r="D50" s="105"/>
+      <c r="E50" s="106"/>
+      <c r="F50" s="104"/>
+      <c r="G50" s="105"/>
+      <c r="H50" s="107"/>
+      <c r="I50" s="108"/>
+      <c r="J50" s="108"/>
+      <c r="K50" s="109"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="6"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+    </row>
+    <row r="52" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="121">
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="H40:K40"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="H38:K38"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="H45:K45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:K34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:K35"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B36:M36"/>
-    <mergeCell ref="H43:K43"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="H44:K44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="B41:M41"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:K33"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:K26"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:K24"/>
-    <mergeCell ref="B23:M23"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:K20"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:K22"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="H16:K16"/>
-    <mergeCell ref="B17:M17"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="O6:O15"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="H8:K8"/>
+  <mergeCells count="133">
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="H9:K9"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:K5"/>
@@ -3249,6 +3315,117 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="H14:K14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:K15"/>
+    <mergeCell ref="O6:O19"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:K13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="H16:K16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:K22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B27:M27"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:K24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:K26"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H33:K33"/>
+    <mergeCell ref="B45:M45"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:K36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:K34"/>
+    <mergeCell ref="H35:K35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:K38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B40:M40"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="H48:K48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="H44:K44"/>
+    <mergeCell ref="H41:K41"/>
+    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H43:K43"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>